<commit_message>
-adds more fields to event annotation
-shiifts event annotation position
</commit_message>
<xml_diff>
--- a/doc/help_dialogs/Input_files/eventannotations.xlsx
+++ b/doc/help_dialogs/Input_files/eventannotations.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="45" windowWidth="11475" windowHeight="5955" activeTab="1"/>
+    <workbookView xWindow="480" yWindow="45" windowWidth="11475" windowHeight="5955"/>
   </bookViews>
   <sheets>
     <sheet name="Annotations" sheetId="1" r:id="rId1"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="58">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="67">
   <si>
     <t>EVENT ANNOTATIONS</t>
   </si>
@@ -190,6 +190,33 @@
   </si>
   <si>
     <t>{20Fresh Cut Grass|50Hay|80Baking Bread|100A Point} @~Y2~degmode</t>
+  </si>
+  <si>
+    <t>~descr</t>
+  </si>
+  <si>
+    <t>The Description field of the Event</t>
+  </si>
+  <si>
+    <t>Gas 10</t>
+  </si>
+  <si>
+    <t>~type</t>
+  </si>
+  <si>
+    <t>The Type field of the Event</t>
+  </si>
+  <si>
+    <t>Power</t>
+  </si>
+  <si>
+    <t>~sldrunit</t>
+  </si>
+  <si>
+    <t>The value of the Slider Unit for this Event</t>
+  </si>
+  <si>
+    <t>kPa</t>
   </si>
 </sst>
 </file>
@@ -544,10 +571,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C15"/>
+  <dimension ref="A1:C18"/>
   <sheetViews>
-    <sheetView topLeftCell="A9" workbookViewId="0">
-      <selection activeCell="A14" sqref="A14"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A9" sqref="A9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -606,106 +633,139 @@
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
-        <v>6</v>
+        <v>58</v>
       </c>
       <c r="B6" t="s">
-        <v>7</v>
-      </c>
-      <c r="C6">
-        <v>522</v>
+        <v>59</v>
+      </c>
+      <c r="C6" t="s">
+        <v>60</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
-        <v>8</v>
+        <v>61</v>
       </c>
       <c r="B7" t="s">
-        <v>29</v>
-      </c>
-      <c r="C7">
-        <v>47</v>
+        <v>62</v>
+      </c>
+      <c r="C7" t="s">
+        <v>63</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
-        <v>9</v>
+        <v>64</v>
       </c>
       <c r="B8" t="s">
-        <v>30</v>
-      </c>
-      <c r="C8">
-        <v>50</v>
+        <v>65</v>
+      </c>
+      <c r="C8" t="s">
+        <v>66</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="B9" t="s">
-        <v>26</v>
+        <v>7</v>
       </c>
       <c r="C9">
-        <v>12</v>
+        <v>522</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="B10" t="s">
-        <v>12</v>
-      </c>
-      <c r="C10" s="2" t="s">
-        <v>27</v>
+        <v>29</v>
+      </c>
+      <c r="C10">
+        <v>47</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="B11" t="s">
-        <v>14</v>
-      </c>
-      <c r="C11" s="2" t="s">
-        <v>15</v>
+        <v>30</v>
+      </c>
+      <c r="C11">
+        <v>50</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
-        <v>16</v>
+        <v>10</v>
       </c>
       <c r="B12" t="s">
-        <v>17</v>
-      </c>
-      <c r="C12" s="3" t="s">
-        <v>28</v>
+        <v>26</v>
+      </c>
+      <c r="C12">
+        <v>12</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
-        <v>18</v>
+        <v>11</v>
       </c>
       <c r="B13" t="s">
-        <v>19</v>
+        <v>12</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>20</v>
+        <v>27</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="B14" t="s">
+        <v>14</v>
+      </c>
+      <c r="C14" s="2" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A15" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="B15" t="s">
+        <v>17</v>
+      </c>
+      <c r="C15" s="3" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A16" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="B16" t="s">
+        <v>19</v>
+      </c>
+      <c r="C16" s="2" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A17" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="B14" t="s">
+      <c r="B17" t="s">
         <v>22</v>
       </c>
-      <c r="C14" s="3" t="s">
+      <c r="C17" s="3" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A15" s="1"/>
-      <c r="C15" s="3"/>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A18" s="1"/>
+      <c r="C18" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -716,7 +776,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A9" sqref="A9"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
adds et-ror and bt-ror to special events annotations
</commit_message>
<xml_diff>
--- a/doc/help_dialogs/Input_files/eventannotations.xlsx
+++ b/doc/help_dialogs/Input_files/eventannotations.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="45" windowWidth="11475" windowHeight="5955" activeTab="2"/>
+    <workbookView xWindow="480" yWindow="45" windowWidth="11475" windowHeight="5955"/>
   </bookViews>
   <sheets>
     <sheet name="Annotations" sheetId="1" r:id="rId1"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="68">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="72">
   <si>
     <t>EVENT ANNOTATIONS</t>
   </si>
@@ -220,6 +220,18 @@
   </si>
   <si>
     <t>When annotations overlap to the oint they can not be read, try reducing the value of the 'Allowed Annotation Overlap' found on the Annotations configuration page.  The default value for this etting is 100%.</t>
+  </si>
+  <si>
+    <t>ET RoR value</t>
+  </si>
+  <si>
+    <t>BT RoR value</t>
+  </si>
+  <si>
+    <t>~R2</t>
+  </si>
+  <si>
+    <t>~R1</t>
   </si>
 </sst>
 </file>
@@ -574,9 +586,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C18"/>
+  <dimension ref="A1:C20"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D15" sqref="D15"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -606,7 +620,7 @@
       <c r="B3" t="s">
         <v>32</v>
       </c>
-      <c r="C3">
+      <c r="C3" s="3">
         <v>60</v>
       </c>
     </row>
@@ -617,7 +631,7 @@
       <c r="B4" t="s">
         <v>24</v>
       </c>
-      <c r="C4">
+      <c r="C4" s="3">
         <v>420</v>
       </c>
     </row>
@@ -628,7 +642,7 @@
       <c r="B5" t="s">
         <v>25</v>
       </c>
-      <c r="C5">
+      <c r="C5" s="3">
         <v>372</v>
       </c>
     </row>
@@ -639,7 +653,7 @@
       <c r="B6" t="s">
         <v>59</v>
       </c>
-      <c r="C6" t="s">
+      <c r="C6" s="3" t="s">
         <v>60</v>
       </c>
     </row>
@@ -650,7 +664,7 @@
       <c r="B7" t="s">
         <v>62</v>
       </c>
-      <c r="C7" t="s">
+      <c r="C7" s="3" t="s">
         <v>63</v>
       </c>
     </row>
@@ -661,7 +675,7 @@
       <c r="B8" t="s">
         <v>65</v>
       </c>
-      <c r="C8" t="s">
+      <c r="C8" s="3" t="s">
         <v>66</v>
       </c>
     </row>
@@ -672,7 +686,7 @@
       <c r="B9" t="s">
         <v>7</v>
       </c>
-      <c r="C9">
+      <c r="C9" s="3">
         <v>522</v>
       </c>
     </row>
@@ -683,7 +697,7 @@
       <c r="B10" t="s">
         <v>29</v>
       </c>
-      <c r="C10">
+      <c r="C10" s="3">
         <v>47</v>
       </c>
     </row>
@@ -694,7 +708,7 @@
       <c r="B11" t="s">
         <v>30</v>
       </c>
-      <c r="C11">
+      <c r="C11" s="3">
         <v>50</v>
       </c>
     </row>
@@ -705,7 +719,7 @@
       <c r="B12" t="s">
         <v>26</v>
       </c>
-      <c r="C12">
+      <c r="C12" s="3">
         <v>12</v>
       </c>
     </row>
@@ -744,29 +758,51 @@
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16" s="2" t="s">
-        <v>18</v>
+        <v>71</v>
       </c>
       <c r="B16" t="s">
-        <v>19</v>
-      </c>
-      <c r="C16" s="2" t="s">
-        <v>20</v>
+        <v>68</v>
+      </c>
+      <c r="C16" s="3">
+        <v>10</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="B17" t="s">
+        <v>69</v>
+      </c>
+      <c r="C17" s="3">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A18" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="B18" t="s">
+        <v>19</v>
+      </c>
+      <c r="C18" s="2" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A19" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="B17" t="s">
+      <c r="B19" t="s">
         <v>22</v>
       </c>
-      <c r="C17" s="3" t="s">
+      <c r="C19" s="3" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A18" s="1"/>
-      <c r="C18" s="3"/>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A20" s="1"/>
+      <c r="C20" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -862,7 +898,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:A11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A11" sqref="A11"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
updates to RoR special events annotations
</commit_message>
<xml_diff>
--- a/doc/help_dialogs/Input_files/eventannotations.xlsx
+++ b/doc/help_dialogs/Input_files/eventannotations.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="45" windowWidth="11475" windowHeight="5955"/>
+    <workbookView xWindow="480" yWindow="45" windowWidth="11475" windowHeight="5955" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Annotations" sheetId="1" r:id="rId1"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="72">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="83">
   <si>
     <t>EVENT ANNOTATIONS</t>
   </si>
@@ -222,16 +222,54 @@
     <t>When annotations overlap to the oint they can not be read, try reducing the value of the 'Allowed Annotation Overlap' found on the Annotations configuration page.  The default value for this etting is 100%.</t>
   </si>
   <si>
-    <t>ET RoR value</t>
-  </si>
-  <si>
-    <t>BT RoR value</t>
-  </si>
-  <si>
     <t>~R2</t>
   </si>
   <si>
     <t>~R1</t>
+  </si>
+  <si>
+    <t>ET RoR value
+Displays '--' when the RoR value is not available.</t>
+  </si>
+  <si>
+    <t>BT RoR value
+Shows '--' when the RoR value Is not available.</t>
+  </si>
+  <si>
+    <t>\u00b0C/min</t>
+  </si>
+  <si>
+    <t>ET RoR with units
+Field is hidden when the RoR value is not available.</t>
+  </si>
+  <si>
+    <t>BT RoR with units
+Field is hidden when the RoR value is not available.</t>
+  </si>
+  <si>
+    <t>Gas ~E/10kPh @~Y2~mode and ~R2~degmin</t>
+  </si>
+  <si>
+    <t>~degmin</t>
+  </si>
+  <si>
+    <t>RoR units
+Shorthand for '~deg~mode/min'</t>
+  </si>
+  <si>
+    <t>~R1degmin</t>
+  </si>
+  <si>
+    <t>~R2degmin</t>
+  </si>
+  <si>
+    <t>9.9\u00b0C/min</t>
+  </si>
+  <si>
+    <t>18.2\u00b0C/min</t>
+  </si>
+  <si>
+    <t>Gas 5.0kPh @340F and 32.8\u00b0F/min</t>
   </si>
 </sst>
 </file>
@@ -280,11 +318,14 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -586,10 +627,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C20"/>
+  <dimension ref="A1:C23"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D15" sqref="D15"/>
+    <sheetView topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="C21" sqref="C21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -756,53 +797,86 @@
         <v>28</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A16" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="B16" s="4" t="s">
+        <v>70</v>
+      </c>
+      <c r="C16" s="3">
+        <v>9.9</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A17" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="B17" s="4" t="s">
         <v>71</v>
       </c>
-      <c r="B16" t="s">
-        <v>68</v>
-      </c>
-      <c r="C16" s="3">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A17" s="2" t="s">
-        <v>70</v>
-      </c>
-      <c r="B17" t="s">
-        <v>69</v>
-      </c>
       <c r="C17" s="3">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+        <v>18.2</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A18" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="B18" s="4" t="s">
+        <v>77</v>
+      </c>
+      <c r="C18" s="2" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A19" s="2" t="s">
+        <v>78</v>
+      </c>
+      <c r="B19" s="4" t="s">
+        <v>73</v>
+      </c>
+      <c r="C19" s="3" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A20" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="B20" s="4" t="s">
+        <v>74</v>
+      </c>
+      <c r="C20" s="3" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A21" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="B18" t="s">
+      <c r="B21" t="s">
         <v>19</v>
       </c>
-      <c r="C18" s="2" t="s">
+      <c r="C21" s="2" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A19" s="2" t="s">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A22" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="B19" t="s">
+      <c r="B22" t="s">
         <v>22</v>
       </c>
-      <c r="C19" s="3" t="s">
+      <c r="C22" s="3" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A20" s="1"/>
-      <c r="C20" s="3"/>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A23" s="1"/>
+      <c r="C23" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -811,10 +885,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B9"/>
+  <dimension ref="A1:B10"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A9" sqref="A9"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -867,25 +941,33 @@
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>47</v>
+        <v>75</v>
       </c>
       <c r="B7" t="s">
-        <v>42</v>
+        <v>82</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B8" t="s">
-        <v>37</v>
+        <v>42</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
+        <v>48</v>
+      </c>
+      <c r="B9" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
         <v>57</v>
       </c>
-      <c r="B9" t="s">
+      <c r="B10" t="s">
         <v>41</v>
       </c>
     </row>

</xml_diff>